<commit_message>
Added content in excel files
</commit_message>
<xml_diff>
--- a/New folder/triaging_template_Rule_016-User added to Microsoft Entra ID Privileged Groups_enhanced.xlsx
+++ b/New folder/triaging_template_Rule_016-User added to Microsoft Entra ID Privileged Groups_enhanced.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anekant.jain\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Agentic AI\Projects\soc\triaging_template\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFAD520-8BFA-4DA0-8E2A-2BDFD22A0A53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F426A142-A03F-4A2A-85A5-EC8A1A7F893A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21912" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Step</t>
   </si>
@@ -212,6 +212,68 @@
   </si>
   <si>
     <t>Azure AD audit logs for privileged role assignments within last 7 days to identify high-risk roles like Global Admin and document assigned users.</t>
+  </si>
+  <si>
+    <t>TimeGenerated            AssignedUser              RoleName                   Initiator              Result
+2025-10-09 10:45:58     emma.wilson@abc.com       Global Administrator       it.admin@abc.com       Success
+2025-10-09 08:45:58     david.brown@abc.com       Privileged Role Admin      security.lead@abc.com  Success  
+2025-10-09 06:45:58     lisa.garcia@abc.com       Security Administrator     it.admin@abc.com       Success
+2025-10-09 03:45:58     robert.jones@abc.com      Exchange Administrator     exchange.admin@abc.com Success</t>
+  </si>
+  <si>
+    <t>TimeGenerated            Username                  GroupName                  AddedBy                IPAddress     Location
+2025-10-09 10:45:58     emma.wilson@abc.com       Global Administrators      it.admin@abc.com       172.16.1.100  New York, NY, US
+2025-10-09 08:45:58     david.brown@abc.com       Privileged Role Admins     security.lead@abc.com  172.16.2.50   Chicago, IL, US
+2025-10-09 06:45:58     lisa.garcia@abc.com       Security Administrators    it.admin@abc.com       172.16.1.100  New York, NY, US
+2025-10-09 03:45:58     robert.jones@abc.com      Exchange Administrators    exchange.admin@abc.com 172.16.3.75   Dallas, TX, US</t>
+  </si>
+  <si>
+    <t>UserPrincipalName        AssignedRole               RiskLevel  RequiresApproval  BusinessJustification                    IsHighRisk
+emma.wilson@abc.com      Global Administrator       Critical   True              Temporary admin access for migration    True
+david.brown@abc.com      Privileged Role Admin      High       True              PIM role for security operations        True
+lisa.garcia@abc.com      Security Administrator     Medium     False             Standard security analyst role          False
+robert.jones@abc.com     Exchange Administrator     Medium     False             Exchange maintenance duties             False</t>
+  </si>
+  <si>
+    <t>UserPrincipalName        SignInCount  UniqueIPs  UniqueLocations  FailedSignIns  Locations                    IPs                              RiskScore
+emma.wilson@abc.com      45          3          2                2              New York, NY; Boston, MA    172.16.1.100; 203.0.113.25      12
+david.brown@abc.com      32          2          1                0              Chicago, IL                  172.16.2.50; 10.0.1.25          6
+lisa.garcia@abc.com      67          1          1                1              New York, NY                 172.16.1.100                     8
+robert.jones@abc.com     28          4          3                5              Dallas, TX; Austin, TX       172.16.3.75; 192.0.2.100        27</t>
+  </si>
+  <si>
+    <t>TimeGenerated            InitiatedBy              OperationName             TargetUser              InitiatorRole            SourceIP      AuthenticationMethod     Result
+2025-10-09 10:45:58     it.admin@abc.com         Add member to role        emma.wilson@abc.com     Global Administrator     172.16.1.100  MFA + Smart Card        Success
+2025-10-09 08:45:58     security.lead@abc.com    Add eligible member       david.brown@abc.com     Privileged Role Admin    172.16.2.50   MFA + Authenticator     Success
+2025-10-09 06:45:58     it.admin@abc.com         Add member to role        lisa.garcia@abc.com     Global Administrator     172.16.1.100  MFA + Smart Card        Success
+2025-10-09 03:45:58     exchange.admin@abc.com   Add member to role        robert.jones@abc.com    Exchange Administrator   172.16.3.75   Password Only           Success</t>
+  </si>
+  <si>
+    <t>UserPrincipalName        SuspiciousActivity                    ThreatIndicators              VirusTotalResult                             RequiresScreenshot  ThreatLevel
+emma.wilson@abc.com      Multiple location sign-ins in 1hr    Impossible travel detected    Clean - No malicious indicators              True               Medium
+david.brown@abc.com      No suspicious activity detected       None                          Clean - No malicious indicators              False              Low
+robert.jones@abc.com     Failed sign-ins from unknown IPs     Brute force attempt           Flagged - 2 vendors marked IP suspicious    True               High</t>
+  </si>
+  <si>
+    <t>UserPrincipalName        ActionTaken                          SessionsRevoked  MFAStatus                  ITNotified  IAMNotified  ComplianceStatus
+emma.wilson@abc.com      Account review initiated             0               Enabled - Authenticator    True        True         Under Review
+david.brown@abc.com      No action required                   0               Enabled - SMS + App        False       False        Compliant
+lisa.garcia@abc.com      Standard monitoring                  0               Enabled - Smart Card       False       False        Compliant
+robert.jones@abc.com     Session revoked, password reset      5               Disabled - Requires setup  True        True         Non-Compliant</t>
+  </si>
+  <si>
+    <t>InvestigationID  UserPrincipalName        ITContactStatus                    IAMVerificationStatus                CredentialResetRequired  FollowUpAction
+PRIV-2025-001    emma.wilson@abc.com      Contacted - Awaiting verification  Verified - Legitimate business need  False                   Monitor for 48 hours
+PRIV-2025-002    david.brown@abc.com      Not required                       Auto-approved - Standard role        False                   No follow-up required
+PRIV-2025-003    lisa.garcia@abc.com      Not required                       Auto-approved - Standard role        False                   No follow-up required
+PRIV-2025-004    robert.jones@abc.com     Contacted - Credential reset       Failed verification - Unauthorized   True                    Full account audit initiated</t>
+  </si>
+  <si>
+    <t>InvestigationID  UserAffected             FindingsSummary                                      RemediationActions                                     Status                   AssignedAnalyst
+PRIV-2025-001    emma.wilson@abc.com      Legitimate assignment requiring monitoring           Enable additional monitoring, require approval        In Progress - Monitoring L2-Analyst-02
+PRIV-2025-002    david.brown@abc.com      Standard privileged role - no issues found          No action required - maintain current access          Closed - No Action       L1-Analyst-04
+PRIV-2025-003    lisa.garcia@abc.com      Security role assignment approved and compliant     No action required - maintain current access          Closed - No Action       L1-Analyst-05
+PRIV-2025-004    robert.jones@abc.com     Unauthorized privileged access - critical finding   Remove access, reset credentials, enable strict CAP   Active - Critical        L3-Analyst-01</t>
   </si>
 </sst>
 </file>
@@ -635,15 +697,15 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="3" max="3" width="33.77734375" customWidth="1"/>
     <col min="4" max="4" width="65" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
@@ -684,7 +746,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="144" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -698,10 +760,12 @@
         <v>9</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -715,10 +779,12 @@
         <v>12</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="F4" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="156" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -732,10 +798,12 @@
         <v>15</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="288" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -749,10 +817,12 @@
         <v>18</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="F6" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -766,10 +836,12 @@
         <v>21</v>
       </c>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="276" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -783,10 +855,12 @@
         <v>24</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -800,10 +874,12 @@
         <v>27</v>
       </c>
       <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="108" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="360" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -817,10 +893,12 @@
         <v>30</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="300" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -834,10 +912,12 @@
         <v>32</v>
       </c>
       <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="132" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -851,7 +931,9 @@
         <v>35</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="G12" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Everything working fine till now
</commit_message>
<xml_diff>
--- a/New folder/triaging_template_Rule_016-User added to Microsoft Entra ID Privileged Groups_enhanced.xlsx
+++ b/New folder/triaging_template_Rule_016-User added to Microsoft Entra ID Privileged Groups_enhanced.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Agentic AI\Projects\soc\triaging_template\New folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F426A142-A03F-4A2A-85A5-EC8A1A7F893A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E4C9EC-035F-4C6B-A63D-E56526094024}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21912" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -391,6 +391,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,20 +699,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="33.77734375" customWidth="1"/>
-    <col min="4" max="4" width="65" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="40" customWidth="1"/>
+    <col min="1" max="1" width="8" style="7" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="23.77734375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="63" style="7" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="56.33203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="40" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -735,7 +739,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>7</v>
@@ -746,7 +750,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="156" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -765,7 +769,7 @@
       </c>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="144" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -784,7 +788,7 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="388.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -803,7 +807,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="288" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -822,7 +826,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="216" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -841,7 +845,7 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="276" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>6</v>
       </c>
@@ -860,7 +864,7 @@
       </c>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="345.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -879,7 +883,7 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="360" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -898,7 +902,7 @@
       </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="324" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -917,7 +921,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -938,5 +942,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>